<commit_message>
Add vs1053 plugin binaries
</commit_message>
<xml_diff>
--- a/Synkino_KiCAD/BOM.xlsx
+++ b/Synkino_KiCAD/BOM.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peaceman/code/Arduino/Synkino/Synkino_KiCAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1BD484-C61A-524A-81CA-22F9D378AC36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD2791D-330F-D94E-9976-A00958DD91FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="3880" windowWidth="28040" windowHeight="21420" xr2:uid="{62282191-527B-B346-A9D5-F4127A77306C}"/>
+    <workbookView xWindow="0" yWindow="4740" windowWidth="33120" windowHeight="26400" xr2:uid="{62282191-527B-B346-A9D5-F4127A77306C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Synkino_BOM" localSheetId="0">Sheet1!$A$1:$E$48</definedName>
+    <definedName name="Synkino_BOM" localSheetId="0">Sheet1!$A$1:$E$50</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="179">
   <si>
     <t>Ref</t>
   </si>
@@ -135,15 +135,6 @@
     <t>LEDs:LED_0805_HandSoldering</t>
   </si>
   <si>
-    <t xml:space="preserve">J1, </t>
-  </si>
-  <si>
-    <t>Conn_01x02_Male</t>
-  </si>
-  <si>
-    <t>Connectors_Molex:Molex_KK-6410-02_02x2.54mm_Straight</t>
-  </si>
-  <si>
     <t xml:space="preserve">J2, J12, </t>
   </si>
   <si>
@@ -180,12 +171,6 @@
     <t>Pin_Headers:Pin_Header_Straight_1x03_Pitch2.54mm</t>
   </si>
   <si>
-    <t xml:space="preserve">JP1, </t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x02_Pitch2.54mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Q1, </t>
   </si>
   <si>
@@ -270,18 +255,9 @@
     <t>22k</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1, SW3, </t>
-  </si>
-  <si>
-    <t>SW_Push</t>
-  </si>
-  <si>
     <t>Buttons_Switches_THT:SW_PUSH_6mm_h5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">SW2, </t>
-  </si>
-  <si>
     <t>Rotary_Encoder_Switch</t>
   </si>
   <si>
@@ -405,9 +381,6 @@
     <t>Mouser Part</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>603-RC0805FR-07300KL</t>
   </si>
   <si>
@@ -468,12 +441,6 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>700-MAX4741EKA+T</t>
-  </si>
-  <si>
-    <t>556-ATMEGA328PB-AN</t>
-  </si>
-  <si>
     <t>512-QRE1113GR</t>
   </si>
   <si>
@@ -501,9 +468,6 @@
     <t>80-C0805C105M4V</t>
   </si>
   <si>
-    <t>80-C0805C104K3RACTM</t>
-  </si>
-  <si>
     <t>80-C0805C473K5R</t>
   </si>
   <si>
@@ -550,6 +514,75 @@
   </si>
   <si>
     <t>alternativer Stecker</t>
+  </si>
+  <si>
+    <t>in stock</t>
+  </si>
+  <si>
+    <t>Encoder Kappe</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/5pcs-lot-LXN17x14-Mini-Aluminum-Alloy-Knobs-Cap-17x14mm-Mounting-6mm-Black-For-Rotary-potentiometer/32843175222.html?spm=a2g0s.9042311.0.0.MeQhJ3</t>
+  </si>
+  <si>
+    <t>needed for 100 kits</t>
+  </si>
+  <si>
+    <t>Kabel 2.5mm</t>
+  </si>
+  <si>
+    <t>open @ Ali</t>
+  </si>
+  <si>
+    <t>open @ Mouser</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>IRML2244</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>SZBX84C9V1LT3G</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW_Push Reset</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW_Push Power</t>
+  </si>
+  <si>
+    <t>863-SZBZX84C9V1LT3G</t>
+  </si>
+  <si>
+    <t>700-MAX4741EUA</t>
+  </si>
+  <si>
+    <t>556-ATMEGA328-AU</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>80-C0805C104Z4V</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>dirtyPCB</t>
   </si>
 </sst>
 </file>
@@ -598,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,6 +642,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,11 +963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A9E284-C181-8342-A542-2F59AD3744EA}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,9 +978,11 @@
     <col min="4" max="4" width="57.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -961,15 +999,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -981,10 +1031,25 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="3">
+        <f>B2*100</f>
+        <v>700</v>
+      </c>
+      <c r="H2">
+        <f>71*7+92</f>
+        <v>589</v>
+      </c>
+      <c r="J2">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K2" t="str">
+        <f>IF(G2-(SUM(H2:J2))&gt;0,G2-H2-I2-J2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -998,10 +1063,21 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G54" si="0">B3*100</f>
+        <v>400</v>
+      </c>
+      <c r="H3">
+        <v>500</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K54" si="1">IF(G3-(SUM(H3:J3))&gt;0,G3-H3-I3-J3,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1015,10 +1091,21 @@
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1032,10 +1119,21 @@
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1049,10 +1147,21 @@
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1066,10 +1175,21 @@
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1083,10 +1203,21 @@
         <v>6</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1100,10 +1231,25 @@
         <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="H9">
+        <f>9*18</f>
+        <v>162</v>
+      </c>
+      <c r="J9">
+        <v>1800</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1117,10 +1263,21 @@
         <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1134,10 +1291,21 @@
         <v>25</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1150,174 +1318,302 @@
       <c r="D12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>180</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="F15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="F16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>48</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
       <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="F18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H18">
+        <v>108</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="F19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="F21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>100</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B22">
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="H22">
+        <v>1400</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1326,32 +1622,54 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1360,32 +1678,54 @@
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H25">
+        <v>200</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1394,49 +1734,82 @@
         <v>470</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H27">
+        <v>200</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H28">
+        <v>200</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" s="4">
-        <v>270</v>
+        <v>680</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H29">
+        <v>1000</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -1445,329 +1818,645 @@
         <v>220</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="H30">
+        <v>800</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="H31">
+        <v>800</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="H32">
+        <v>600</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H33">
+        <v>200</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>50</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>40</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H37">
+        <f>40+10</f>
+        <v>50</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="D33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="D38" t="s">
         <v>74</v>
       </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="F38" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>50</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D34" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>76</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="D39" t="s">
         <v>77</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="F39" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H39" s="6">
+        <v>110</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D35" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="D40" t="s">
         <v>80</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E40" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>10</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D36" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="D41" t="s">
         <v>83</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="F41" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D37" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="D42" t="s">
         <v>86</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="F42" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H42" s="6">
+        <v>108</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D38" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>88</v>
       </c>
-      <c r="E38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="D43" t="s">
         <v>89</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="E43" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>16</v>
+      </c>
+      <c r="I43">
+        <f>50+10</f>
+        <v>60</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D39" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="D44" t="s">
         <v>92</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="F44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>42</v>
+      </c>
+      <c r="I44">
+        <v>24</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D40" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" t="s">
-        <v>100</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44">
-        <v>8</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H45">
+        <v>51</v>
+      </c>
+      <c r="J45">
+        <v>25</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>104</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H49" s="6">
+        <v>220</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D45" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46">
+      <c r="D50" t="s">
+        <v>107</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H50">
+        <v>10</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>152</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B53">
         <v>2</v>
       </c>
-      <c r="C46" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" t="s">
-        <v>115</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>117</v>
-      </c>
-      <c r="D48" t="s">
-        <v>115</v>
-      </c>
-      <c r="F48" s="3" t="s">
+      <c r="D53" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="4:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
-        <v>167</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>166</v>
+      <c r="G53" s="3">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" t="s">
+        <v>178</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H54">
+        <v>11</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>